<commit_message>
regression model for strength prediction
</commit_message>
<xml_diff>
--- a/XG_BoostRegressor2.xlsx
+++ b/XG_BoostRegressor2.xlsx
@@ -465,19 +465,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8545324398721323</v>
+        <v>0.7911308369771046</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9759101288197498</v>
+        <v>0.8529849757961881</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9858375497188395</v>
+        <v>0.8843807794783712</v>
       </c>
       <c r="E2" t="n">
-        <v>0.790989232068618</v>
+        <v>0.6145278463798798</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9204927157693231</v>
+        <v>0.8336114287689569</v>
       </c>
     </row>
     <row r="3">
@@ -491,7 +491,8 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RandomForestRegressor(bootstrap=False, max_features='sqrt', n_estimators=10)</t>
+          <t>RandomForestRegressor(bootstrap=False, max_features='log2', min_samples_split=8,
+                      n_estimators=20)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -499,8 +500,8 @@
           <t>XGBRegressor(base_score=0.5, booster='gbtree', colsample_bylevel=1,
              colsample_bynode=1, colsample_bytree=1, gamma=0, gpu_id=-1,
              importance_type='gain', interaction_constraints='',
-             learning_rate=0.1, max_delta_step=0, max_depth=10,
-             min_child_weight=1, missing=nan, monotone_constraints='()',
+             learning_rate=0.1, max_delta_step=0, max_depth=2,
+             min_child_weight=3, missing=nan, monotone_constraints='()',
              n_estimators=100, n_jobs=2, num_parallel_tree=1, random_state=0,
              reg_alpha=0, reg_lambda=1, scale_pos_weight=1, subsample=1,
              tree_method='exact', validate_parameters=1, verbosity=None)</t>
@@ -508,12 +509,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>DecisionTreeRegressor(max_depth=8, min_samples_leaf=20, min_samples_split=10)</t>
+          <t>DecisionTreeRegressor(max_depth=6, min_samples_leaf=20, min_samples_split=20)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>AdaBoostRegressor(learning_rate=0.1, n_estimators=2000, random_state=1)</t>
+          <t>AdaBoostRegressor(learning_rate=0.01, n_estimators=2000, random_state=1)</t>
         </is>
       </c>
     </row>
@@ -522,19 +523,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>37.42997115269382</v>
+        <v>51.28397524569497</v>
       </c>
       <c r="C4" t="n">
-        <v>6.198517267741935</v>
+        <v>36.0968309198763</v>
       </c>
       <c r="D4" t="n">
-        <v>3.64411216500319</v>
+        <v>28.38816969122341</v>
       </c>
       <c r="E4" t="n">
-        <v>53.78014869705155</v>
+        <v>94.64558625148524</v>
       </c>
       <c r="F4" t="n">
-        <v>20.45786258164614</v>
+        <v>40.85364849785898</v>
       </c>
     </row>
     <row r="5">
@@ -542,19 +543,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>4.357283377887136</v>
+        <v>5.509141880637524</v>
       </c>
       <c r="C5" t="n">
-        <v>1.632512903225807</v>
+        <v>4.626085546398045</v>
       </c>
       <c r="D5" t="n">
-        <v>1.109204682503977</v>
+        <v>3.450379840899736</v>
       </c>
       <c r="E5" t="n">
-        <v>4.53835437394299</v>
+        <v>7.147151009713077</v>
       </c>
       <c r="F5" t="n">
-        <v>3.666680803199678</v>
+        <v>4.950831660752229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>